<commit_message>
going back to original file of qzap records
and whatever else happened since the last commit
</commit_message>
<xml_diff>
--- a/records_maps/Capstone Maps/denver-map2019.xlsx
+++ b/records_maps/Capstone Maps/denver-map2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfreedma/Documents/GitHub/zinecat.org/records_maps/Capstone Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC55C95D-2F87-C24C-81E8-0E053EA0A5CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F2CAD3-4E14-3B4B-89E9-A223EF303D70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="2080" windowWidth="19080" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6140" yWindow="1500" windowWidth="19080" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="100">
   <si>
     <t>Rule Type</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Set to yes to save the data spreadsheet or no to delete it from the server after import</t>
   </si>
   <si>
-    <t>{ "relationshipType": "publisher", "entityType": "org"}</t>
-  </si>
-  <si>
     <t>ca_objects.altID</t>
   </si>
   <si>
@@ -319,6 +316,15 @@
   </si>
   <si>
     <t>ca_objects.date.datetext</t>
+  </si>
+  <si>
+    <t>ca_objects.subtitle</t>
+  </si>
+  <si>
+    <t>{ "relationshipType": "creator", "entityType": "org"}</t>
+  </si>
+  <si>
+    <t>ca_objects.format_text</t>
   </si>
 </sst>
 </file>
@@ -757,8 +763,8 @@
   </sheetPr>
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -864,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -875,10 +881,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="34" x14ac:dyDescent="0.2">
@@ -895,24 +901,24 @@
         <v>52</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B8" s="9">
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -929,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -946,7 +952,7 @@
         <v>53</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -957,13 +963,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -974,13 +980,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -991,13 +997,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1053,7 +1059,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>30</v>
@@ -1070,13 +1076,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1095,7 +1101,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1106,7 +1112,7 @@
         <v>62</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1238,7 +1244,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>